<commit_message>
Tested excel function from the tutorials. Except some minor problems, all is well.
</commit_message>
<xml_diff>
--- a/UserExperience.xlsx
+++ b/UserExperience.xlsx
@@ -2,24 +2,24 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
-  <workbookPr/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\adrian.alecu\VAAS\VAASDoc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9228" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9228"/>
   </bookViews>
   <sheets>
-    <sheet name="Nice to have 2017_02_02" sheetId="6" r:id="rId1"/>
+    <sheet name="Nice to have 2017_02_17" sheetId="6" r:id="rId1"/>
     <sheet name="Nice to have 2017_01_19" sheetId="5" r:id="rId2"/>
     <sheet name="Nice to have 2017_01_12" sheetId="2" r:id="rId3"/>
     <sheet name="Help!!!" sheetId="4" r:id="rId4"/>
     <sheet name="Questions" sheetId="1" r:id="rId5"/>
     <sheet name="FirstWorkflow Diagram" sheetId="3" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="106">
   <si>
     <t>It would be nice to have a state of the tutorial - it exists in the instance but it dissapears when you close it. It should be account related.</t>
   </si>
@@ -497,6 +497,88 @@
       </rPr>
       <t>&gt;&gt;&gt; Yes, there is a significant impact when you properly build your script. You need circa 30s to get prices in both simulations, with and without parallelization of the market data inputs. I have rebuilt your script and I get 8.966s to get prices with parallelized scenario values against 11.464s without. Enclosed, please find the script and results.</t>
     </r>
+  </si>
+  <si>
+    <t>The operation is ok when using a new empty sheet</t>
+  </si>
+  <si>
+    <t>When transforming the item, points should be centered up, else the scrolling can get long.</t>
+  </si>
+  <si>
+    <t>First try - paste Json from cliboard the dev environement into Market Data Values: JPY10MD156N.json - the pasted json should start from the selected cell</t>
+  </si>
+  <si>
+    <t>The videos - you should redo them, the quality of the sound is quite bad</t>
+  </si>
+  <si>
+    <t>The functions should have help on arguments:</t>
+  </si>
+  <si>
+    <t>I think it is important to state that every FFP object is a Json and you can do a FppCommandViewJson to get more information</t>
+  </si>
+  <si>
+    <t>I am trying to use the function FppFromJson without any success I have passed the string {
+    ""PriceIndex"": [
+     ""ONTD156N""
+    ]
+}</t>
+  </si>
+  <si>
+    <t>In the tutorial there should be the information of which call is connecting to the server, =FppRetrieveLibraryContent(B8) - does not work stand alone and I had to copy the full ServerConfig page to connect</t>
+  </si>
+  <si>
+    <t>{</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "errors": [],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "traceLog": [],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "results": [</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      "values": [</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        []</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      ],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      "type": "ARRAY"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ]</t>
+  </si>
+  <si>
+    <t>}</t>
+  </si>
+  <si>
+    <t>I think you need to add some framework debuging messages, I call pricer, it gets somewhere but I have no clue what happends:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      "id": "622be1ca-1e3b-472a-95a1-6082c7978be3",</t>
+  </si>
+  <si>
+    <t>You need to have a shortcut key to ViewJson</t>
+  </si>
+  <si>
+    <t>The videos - the one that is doing them should write from 0, not delete and type the same text that was already there (give the impression that its a training)</t>
+  </si>
+  <si>
+    <t>The users need excel examples with each function used (just like the ones that exist but for all functions). Ex: on a client, when you wrote a function, you also did an excel with an example of how to use the function and also you wrote the list of parameters with a small statement.</t>
+  </si>
+  <si>
+    <t>How to user FppData1D to get a multi scenario array?</t>
   </si>
 </sst>
 </file>
@@ -602,14 +684,14 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -641,8 +723,8 @@
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>315686</xdr:colOff>
-      <xdr:row>73</xdr:row>
-      <xdr:rowOff>137160</xdr:rowOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>104502</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -677,6 +759,178 @@
         </a:extLst>
       </xdr:spPr>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>5421086</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>21773</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>11181806</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>170363</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Image 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{15A50F00-F4CD-4FDD-B587-43F870C0EAC5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5421086" y="576944"/>
+          <a:ext cx="5760720" cy="2739390"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>21771</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>43543</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>4241346</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Image 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2B436414-2C16-46E7-A688-288F2E32BC4D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="21771" y="598714"/>
+          <a:ext cx="4219575" cy="2457450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>8019048</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>176533</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Image 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E514562-62DD-42A1-B106-861F00A933A8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="3777343"/>
+          <a:ext cx="8019048" cy="2876190"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>6714286</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>112485</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Image 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{525ABBC6-9162-4D03-B99C-00716737E684}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="7957457"/>
+          <a:ext cx="6714286" cy="3628571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1345,10 +1599,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A15:A69"/>
+  <sheetPr codeName="Feuil1"/>
+  <dimension ref="A1:A90"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A98" sqref="A98"/>
+    <sheetView tabSelected="1" topLeftCell="A68" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A91" sqref="A91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -1356,6 +1611,16 @@
     <col min="1" max="1" width="255.77734375" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>80</v>
+      </c>
+    </row>
     <row r="15" spans="1:1">
       <c r="A15" s="4"/>
     </row>
@@ -1365,6 +1630,11 @@
     <row r="18" spans="1:1">
       <c r="A18" s="4"/>
     </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>81</v>
+      </c>
+    </row>
     <row r="21" spans="1:1">
       <c r="A21" s="5"/>
     </row>
@@ -1386,80 +1656,180 @@
     <row r="37" spans="1:1">
       <c r="A37" s="6"/>
     </row>
+    <row r="39" spans="1:1">
+      <c r="A39" t="s">
+        <v>83</v>
+      </c>
+    </row>
     <row r="40" spans="1:1">
       <c r="A40" s="6"/>
     </row>
     <row r="41" spans="1:1">
-      <c r="A41" s="6"/>
+      <c r="A41" s="6" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="43" spans="1:1">
-      <c r="A43" s="6"/>
+      <c r="A43" s="6" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45" s="6"/>
     </row>
     <row r="48" spans="1:1">
-      <c r="A48" s="8"/>
+      <c r="A48" s="7"/>
     </row>
     <row r="50" spans="1:1">
-      <c r="A50" s="8"/>
+      <c r="A50" s="7"/>
     </row>
     <row r="51" spans="1:1">
-      <c r="A51" s="8"/>
+      <c r="A51" s="7"/>
     </row>
     <row r="52" spans="1:1">
-      <c r="A52" s="8"/>
+      <c r="A52" s="7"/>
     </row>
     <row r="53" spans="1:1">
-      <c r="A53" s="8"/>
+      <c r="A53" s="7"/>
     </row>
     <row r="54" spans="1:1">
-      <c r="A54" s="8"/>
+      <c r="A54" s="7"/>
     </row>
     <row r="55" spans="1:1">
-      <c r="A55" s="8"/>
+      <c r="A55" s="7"/>
     </row>
     <row r="56" spans="1:1">
-      <c r="A56" s="8"/>
+      <c r="A56" s="7"/>
     </row>
     <row r="57" spans="1:1">
-      <c r="A57" s="8"/>
+      <c r="A57" s="7"/>
     </row>
     <row r="58" spans="1:1">
-      <c r="A58" s="8"/>
+      <c r="A58" s="7"/>
     </row>
     <row r="59" spans="1:1">
-      <c r="A59" s="8"/>
+      <c r="A59" s="7"/>
     </row>
     <row r="60" spans="1:1">
-      <c r="A60" s="8"/>
+      <c r="A60" s="7"/>
     </row>
     <row r="61" spans="1:1">
-      <c r="A61" s="9"/>
+      <c r="A61" s="8"/>
     </row>
     <row r="62" spans="1:1">
       <c r="A62" s="5"/>
     </row>
     <row r="63" spans="1:1">
-      <c r="A63" s="8"/>
+      <c r="A63" s="7"/>
     </row>
     <row r="64" spans="1:1">
-      <c r="A64" s="8"/>
+      <c r="A64" s="7" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="65" spans="1:1">
-      <c r="A65" s="9"/>
+      <c r="A65" s="8"/>
     </row>
     <row r="66" spans="1:1">
-      <c r="A66" s="9"/>
-    </row>
-    <row r="67" spans="1:1">
-      <c r="A67" s="8"/>
+      <c r="A66" s="7" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" ht="61.2">
+      <c r="A67" s="7" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="68" spans="1:1">
-      <c r="A68" s="8"/>
+      <c r="A68" s="7"/>
     </row>
     <row r="69" spans="1:1">
-      <c r="A69" s="8"/>
+      <c r="A69" s="7"/>
+    </row>
+    <row r="70" spans="1:1">
+      <c r="A70" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1">
+      <c r="A72" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1">
+      <c r="A73" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1">
+      <c r="A74" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1">
+      <c r="A75" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1">
+      <c r="A76" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1">
+      <c r="A77" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1">
+      <c r="A78" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1">
+      <c r="A79" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1">
+      <c r="A80" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1">
+      <c r="A81" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1">
+      <c r="A82" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1">
+      <c r="A83" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1">
+      <c r="A84" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1">
+      <c r="A85" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1">
+      <c r="A88" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1">
+      <c r="A90" t="s">
+        <v>105</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1470,9 +1840,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Feuil2"/>
   <dimension ref="A1:A69"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="A74" sqref="A74"/>
     </sheetView>
   </sheetViews>
@@ -1573,108 +1944,108 @@
         <v>60</v>
       </c>
     </row>
-    <row r="48" spans="1:1" ht="20.399999999999999">
-      <c r="A48" s="8" t="s">
+    <row r="48" spans="1:1">
+      <c r="A48" s="7" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="50" spans="1:1" ht="20.399999999999999">
-      <c r="A50" s="8" t="s">
+    <row r="50" spans="1:1">
+      <c r="A50" s="7" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="51" spans="1:1" ht="20.399999999999999">
-      <c r="A51" s="8" t="s">
+    <row r="51" spans="1:1">
+      <c r="A51" s="7" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="52" spans="1:1" ht="20.399999999999999">
-      <c r="A52" s="8" t="s">
+    <row r="52" spans="1:1">
+      <c r="A52" s="7" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="53" spans="1:1">
-      <c r="A53" s="8" t="s">
+      <c r="A53" s="7" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="54" spans="1:1">
-      <c r="A54" s="8" t="s">
+      <c r="A54" s="7" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="55" spans="1:1">
-      <c r="A55" s="8" t="s">
+      <c r="A55" s="7" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="56" spans="1:1">
-      <c r="A56" s="8" t="s">
+      <c r="A56" s="7" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="57" spans="1:1">
-      <c r="A57" s="8" t="s">
+      <c r="A57" s="7" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="58" spans="1:1">
-      <c r="A58" s="8" t="s">
+      <c r="A58" s="7" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="59" spans="1:1">
-      <c r="A59" s="8" t="s">
+      <c r="A59" s="7" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="60" spans="1:1">
-      <c r="A60" s="8" t="s">
+      <c r="A60" s="7" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="61" spans="1:1" ht="30.6">
-      <c r="A61" s="9" t="s">
+    <row r="61" spans="1:1" ht="20.399999999999999">
+      <c r="A61" s="8" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="62" spans="1:1" ht="28.8">
+    <row r="62" spans="1:1">
       <c r="A62" s="5" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="63" spans="1:1">
-      <c r="A63" s="8" t="s">
+      <c r="A63" s="7" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="64" spans="1:1" ht="20.399999999999999">
-      <c r="A64" s="8" t="s">
+      <c r="A64" s="7" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="65" spans="1:1">
-      <c r="A65" s="9" t="s">
+      <c r="A65" s="8" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="66" spans="1:1" ht="20.399999999999999">
-      <c r="A66" s="9" t="s">
+      <c r="A66" s="8" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="67" spans="1:1">
-      <c r="A67" s="8" t="s">
+      <c r="A67" s="7" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="68" spans="1:1" ht="20.399999999999999">
-      <c r="A68" s="8" t="s">
+      <c r="A68" s="7" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="69" spans="1:1">
-      <c r="A69" s="8"/>
+      <c r="A69" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1685,6 +2056,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Feuil3"/>
   <dimension ref="A1:A35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1818,6 +2190,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Feuil4"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1838,6 +2211,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Feuil5"/>
   <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1888,6 +2262,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Feuil6"/>
   <dimension ref="A3:K21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1911,11 +2286,11 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:11">
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
     </row>
     <row r="4" spans="1:11">
       <c r="D4" s="1" t="s">
@@ -1931,13 +2306,13 @@
       </c>
     </row>
     <row r="8" spans="1:11">
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
     </row>
     <row r="9" spans="1:11">
       <c r="C9" s="1" t="s">
@@ -1998,20 +2373,20 @@
       </c>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="G16" s="7" t="s">
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="G16" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="7"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="1" t="s">
@@ -2033,13 +2408,13 @@
       </c>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="3" t="s">

</xml_diff>